<commit_message>
adding images for data evaluation
</commit_message>
<xml_diff>
--- a/Project-SQL/SQL Data Files/data types.xlsx
+++ b/Project-SQL/SQL Data Files/data types.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clintonboyda/Documents/GitHub/LighthouseLabs/SQL Data Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clintonboyda/Documents/GitHub/LighthouseLabs/Project-SQL/SQL Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13366376-B52D-4C4A-B1C7-115D512779EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A2CB1C2-DC85-D149-B6E2-36017D2A775C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="1560" windowWidth="28040" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16720" yWindow="1520" windowWidth="28040" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datatypes" sheetId="2" r:id="rId1"/>
@@ -2207,7 +2207,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>